<commit_message>
chore: compute distances from provided addresses inside prospect excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/files/prospect-ko-400.xlsx
+++ b/src/main/resources/files/prospect-ko-400.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afryan/IdeaProjects/bpartners-api/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BDB1A7-F77C-394B-95EB-A8420A25FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E326CE-F65C-E846-9325-5E89054AC649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
   <si>
     <t>website</t>
   </si>
@@ -602,9 +602,6 @@
     <t>Nouvelle intervention : adresse de l'intervention</t>
   </si>
   <si>
-    <t>Nouvelle intervention : distance entre l'intervention et le nouveau prospect (en mètres)</t>
-  </si>
-  <si>
     <t>Nouvelle intervention - Ancien client : Type du client</t>
   </si>
   <si>
@@ -614,9 +611,6 @@
     <t>Nouvelle intervention - Ancien client : Adresse de l'ancien client</t>
   </si>
   <si>
-    <t>Nouvelle intervention - Ancien client : Distance entre l'ancien client et la nouvelle intervention</t>
-  </si>
-  <si>
     <t>Nouvelle intervention :  type d'infesation</t>
   </si>
   <si>
@@ -626,13 +620,7 @@
     <t>Cambriolage : adresse du cambriolage</t>
   </si>
   <si>
-    <t>Cambriolage : distance entre le cambriolage et le prospect</t>
-  </si>
-  <si>
     <t>Cambriolage - Ancien client : adresse de l'ancien  client cambriolé</t>
-  </si>
-  <si>
-    <t>Cambriolage - Ancien client : distance entre l'ancien  client cambriolé et le cambriolage</t>
   </si>
   <si>
     <t>15 Rue Marbeuf, 75008 Paris, France</t>
@@ -900,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1021,20 +1009,9 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1277,10 +1254,10 @@
     <tabColor rgb="FF00B050"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AR3"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1302,28 +1279,22 @@
     <col min="21" max="22" width="20.5" customWidth="1"/>
     <col min="23" max="23" width="20.6640625" customWidth="1"/>
     <col min="24" max="24" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21" style="45" customWidth="1"/>
-    <col min="26" max="26" width="24.1640625" customWidth="1"/>
-    <col min="27" max="27" width="20.5" customWidth="1"/>
-    <col min="28" max="28" width="24.1640625" customWidth="1"/>
-    <col min="29" max="29" width="24.1640625" style="44" customWidth="1"/>
-    <col min="30" max="30" width="11.5" style="30" customWidth="1"/>
-    <col min="31" max="31" width="14.5" style="30"/>
-    <col min="32" max="32" width="14.5" style="47"/>
-    <col min="33" max="33" width="14.5" style="30"/>
-    <col min="34" max="34" width="14.5" style="47"/>
-    <col min="35" max="36" width="14.5" style="30"/>
-    <col min="37" max="37" width="22.33203125" style="30" customWidth="1"/>
-    <col min="38" max="38" width="21.5" style="30" customWidth="1"/>
-    <col min="39" max="39" width="23.5" style="30" customWidth="1"/>
-    <col min="40" max="40" width="32.1640625" style="30" customWidth="1"/>
-    <col min="41" max="41" width="51.6640625" style="30" customWidth="1"/>
-    <col min="42" max="42" width="24.1640625" style="30" customWidth="1"/>
-    <col min="43" max="43" width="19.6640625" style="30" customWidth="1"/>
-    <col min="44" max="44" width="30.33203125" style="30" customWidth="1"/>
+    <col min="25" max="25" width="24.1640625" customWidth="1"/>
+    <col min="26" max="26" width="20.5" customWidth="1"/>
+    <col min="27" max="27" width="24.1640625" customWidth="1"/>
+    <col min="28" max="28" width="11.5" style="30" customWidth="1"/>
+    <col min="29" max="32" width="14.5" style="30"/>
+    <col min="33" max="33" width="22.33203125" style="30" customWidth="1"/>
+    <col min="34" max="34" width="21.5" style="30" customWidth="1"/>
+    <col min="35" max="35" width="23.5" style="30" customWidth="1"/>
+    <col min="36" max="36" width="32.1640625" style="30" customWidth="1"/>
+    <col min="37" max="37" width="51.6640625" style="30" customWidth="1"/>
+    <col min="38" max="38" width="24.1640625" style="30" customWidth="1"/>
+    <col min="39" max="39" width="19.6640625" style="30" customWidth="1"/>
+    <col min="40" max="40" width="30.33203125" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40">
         <v>0</v>
       </c>
@@ -1396,38 +1367,26 @@
       <c r="X1" s="40">
         <v>23</v>
       </c>
-      <c r="Y1" s="45">
+      <c r="Y1">
         <v>24</v>
       </c>
       <c r="Z1" s="40">
         <v>25</v>
       </c>
-      <c r="AA1" s="40">
+      <c r="AA1">
         <v>26</v>
       </c>
       <c r="AB1" s="40">
         <v>27</v>
       </c>
-      <c r="AC1" s="45">
+      <c r="AC1">
         <v>28</v>
       </c>
       <c r="AD1" s="40">
         <v>29</v>
       </c>
-      <c r="AE1" s="40">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="45">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="40">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="45">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:40" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>170</v>
       </c>
@@ -1495,7 +1454,7 @@
         <v>177</v>
       </c>
       <c r="W2" s="41" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="X2" s="35" t="s">
         <v>178</v>
@@ -1509,39 +1468,27 @@
       <c r="AA2" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="AB2" s="35" t="s">
-        <v>182</v>
-      </c>
-      <c r="AC2" s="35" t="s">
+      <c r="AB2" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="AD2" s="46" t="s">
+      <c r="AC2" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD2" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="AE2" s="46" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF2" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="AG2" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="AH2" s="46" t="s">
-        <v>189</v>
-      </c>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="31"/>
       <c r="AI2" s="31"/>
       <c r="AJ2" s="31"/>
       <c r="AK2" s="31"/>
       <c r="AL2" s="31"/>
       <c r="AM2" s="31"/>
       <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
-      <c r="AQ2" s="31"/>
-      <c r="AR2" s="31"/>
-    </row>
-    <row r="3" spans="1:44" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:40" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>15</v>
       </c>
@@ -1573,7 +1520,7 @@
       <c r="K3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="51">
+      <c r="L3" s="46">
         <v>44197</v>
       </c>
       <c r="M3" s="39" t="s">
@@ -1597,41 +1544,35 @@
       <c r="U3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="48" t="s">
+      <c r="V3" s="43" t="s">
         <v>90</v>
       </c>
       <c r="W3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y3" s="43">
-        <v>500</v>
-      </c>
+      <c r="X3" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y3" s="28"/>
       <c r="Z3" s="28"/>
       <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="42"/>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="33"/>
+      <c r="AF3" s="33"/>
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="33"/>
       <c r="AI3" s="33"/>
-      <c r="AJ3" s="33"/>
-      <c r="AK3" s="32"/>
-      <c r="AL3" s="33"/>
-      <c r="AM3" s="33"/>
-      <c r="AN3" s="32"/>
-      <c r="AO3" s="34"/>
-      <c r="AP3" s="32"/>
-      <c r="AQ3" s="32"/>
-      <c r="AR3" s="33"/>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="34"/>
+      <c r="AL3" s="32"/>
+      <c r="AM3" s="32"/>
+      <c r="AN3" s="33"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P3 AD3 Q3:T3 U3 I3" xr:uid="{5927C8BD-C5E0-BD4C-9A04-5AA2141EF2DB}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AB3 P3:U3 I3" xr:uid="{5927C8BD-C5E0-BD4C-9A04-5AA2141EF2DB}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3" xr:uid="{8AB4D866-60F3-154F-84DA-A5E5880951E1}">
@@ -1775,7 +1716,7 @@
       </c>
     </row>
     <row r="7" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="47" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -1796,7 +1737,7 @@
       </c>
     </row>
     <row r="8" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C8" s="53"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="11" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1756,7 @@
       </c>
     </row>
     <row r="9" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C9" s="53"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="12" t="s">
         <v>49</v>
       </c>
@@ -1834,7 +1775,7 @@
       </c>
     </row>
     <row r="10" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C10" s="53"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="11" t="s">
         <v>50</v>
       </c>
@@ -1853,7 +1794,7 @@
       </c>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C11" s="53"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1862,7 +1803,7 @@
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C12" s="53"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="13" t="s">
         <v>51</v>
       </c>
@@ -1898,7 +1839,7 @@
       <c r="V12" s="5"/>
     </row>
     <row r="13" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C13" s="53"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="13" t="s">
         <v>55</v>
       </c>
@@ -1934,7 +1875,7 @@
       <c r="V13" s="5"/>
     </row>
     <row r="14" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C14" s="53"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="12" t="s">
         <v>56</v>
       </c>
@@ -1970,7 +1911,7 @@
       <c r="V14" s="5"/>
     </row>
     <row r="15" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C15" s="53"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="11" t="s">
         <v>57</v>
       </c>
@@ -2006,7 +1947,7 @@
       <c r="V15" s="5"/>
     </row>
     <row r="16" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C16" s="54"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="11" t="s">
         <v>59</v>
       </c>
@@ -2122,13 +2063,13 @@
       <c r="I19" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="49" t="s">
+      <c r="J19" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="K19" s="49" t="s">
+      <c r="K19" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="49" t="s">
+      <c r="L19" s="44" t="s">
         <v>91</v>
       </c>
       <c r="M19" s="5"/>
@@ -2225,7 +2166,7 @@
       <c r="V21" s="5"/>
     </row>
     <row r="22" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="47" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -2263,7 +2204,7 @@
       <c r="V22" s="5"/>
     </row>
     <row r="23" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="53"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="16" t="s">
         <v>86</v>
       </c>
@@ -2299,7 +2240,7 @@
       <c r="V23" s="5"/>
     </row>
     <row r="24" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="53"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="16" t="s">
         <v>88</v>
       </c>
@@ -2323,7 +2264,7 @@
       </c>
     </row>
     <row r="25" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="53"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="16" t="s">
         <v>92</v>
       </c>
@@ -2344,7 +2285,7 @@
       </c>
     </row>
     <row r="26" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="54"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="16" t="s">
         <v>96</v>
       </c>
@@ -2419,7 +2360,7 @@
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="52" t="s">
+      <c r="C31" s="47" t="s">
         <v>107</v>
       </c>
       <c r="D31" s="16" t="s">
@@ -2444,7 +2385,7 @@
       </c>
     </row>
     <row r="32" spans="2:31" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="53"/>
+      <c r="C32" s="48"/>
       <c r="D32" s="11" t="s">
         <v>111</v>
       </c>
@@ -2527,7 +2468,7 @@
       </c>
     </row>
     <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="54"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="16" t="s">
         <v>86</v>
       </c>
@@ -2775,7 +2716,7 @@
       <c r="B45" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="52" t="s">
+      <c r="C45" s="47" t="s">
         <v>157</v>
       </c>
       <c r="D45" s="20" t="s">
@@ -2799,7 +2740,7 @@
       </c>
     </row>
     <row r="46" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="53"/>
+      <c r="C46" s="48"/>
       <c r="D46" s="20" t="s">
         <v>163</v>
       </c>
@@ -2821,7 +2762,7 @@
       </c>
     </row>
     <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="54"/>
+      <c r="C47" s="49"/>
       <c r="D47" s="20" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
fix: add validation in excel file for prospect evaluations
</commit_message>
<xml_diff>
--- a/src/main/resources/files/prospect-ko-400.xlsx
+++ b/src/main/resources/files/prospect-ko-400.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afryan/IdeaProjects/bpartners-api/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E326CE-F65C-E846-9325-5E89054AC649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2D14CE-02A1-7E4E-B73D-3ADD31D393C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source Depa1" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="191">
   <si>
     <t>website</t>
   </si>
@@ -625,6 +625,18 @@
   <si>
     <t>15 Rue Marbeuf, 75008 Paris, France</t>
   </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Other infestation</t>
+  </si>
+  <si>
+    <t>Other professionnal</t>
+  </si>
+  <si>
+    <t>Other intervention</t>
+  </si>
 </sst>
 </file>
 
@@ -633,7 +645,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,6 +695,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -741,7 +760,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -884,11 +903,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1012,9 +1066,6 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1023,6 +1074,21 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1256,8 +1322,8 @@
   </sheetPr>
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:AD1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1438,7 +1504,7 @@
       <c r="Q2" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="47" t="s">
         <v>173</v>
       </c>
       <c r="S2" s="26" t="s">
@@ -1453,7 +1519,7 @@
       <c r="V2" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="W2" s="41" t="s">
+      <c r="W2" s="49" t="s">
         <v>182</v>
       </c>
       <c r="X2" s="35" t="s">
@@ -1520,20 +1586,24 @@
       <c r="K3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="46">
+      <c r="L3" s="45">
         <v>44197</v>
       </c>
       <c r="M3" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="38"/>
+      <c r="N3" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="P3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27" t="s">
-        <v>54</v>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="48" t="s">
+        <v>187</v>
       </c>
       <c r="S3" s="27" t="s">
         <v>53</v>
@@ -1544,17 +1614,21 @@
       <c r="U3" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="V3" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="W3" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" s="45" t="s">
+      <c r="V3" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="W3" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="X3" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
+      <c r="Y3" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="AA3" s="28"/>
       <c r="AB3" s="27"/>
       <c r="AC3" s="28"/>
@@ -1572,7 +1646,7 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AB3 P3:U3 I3" xr:uid="{5927C8BD-C5E0-BD4C-9A04-5AA2141EF2DB}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AB3 I3 P3:Q3 S3:U3" xr:uid="{5927C8BD-C5E0-BD4C-9A04-5AA2141EF2DB}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N3" xr:uid="{8AB4D866-60F3-154F-84DA-A5E5880951E1}">
@@ -1583,24 +1657,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90FDC7BB-8344-2344-A75E-150A726B1552}">
-          <x14:formula1>
-            <xm:f>'Spec données croisées Depa'!$J$20:$V$20</xm:f>
-          </x14:formula1>
-          <xm:sqref>W3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{3B96BB93-1342-2649-BEE7-943317411060}">
-          <x14:formula1>
-            <xm:f>'Spec données croisées Depa'!$J$19:$L$19</xm:f>
-          </x14:formula1>
-          <xm:sqref>V3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1716,7 +1772,7 @@
       </c>
     </row>
     <row r="7" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="51" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -1737,7 +1793,7 @@
       </c>
     </row>
     <row r="8" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C8" s="48"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="11" t="s">
         <v>24</v>
       </c>
@@ -1756,7 +1812,7 @@
       </c>
     </row>
     <row r="9" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C9" s="48"/>
+      <c r="C9" s="52"/>
       <c r="D9" s="12" t="s">
         <v>49</v>
       </c>
@@ -1775,7 +1831,7 @@
       </c>
     </row>
     <row r="10" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C10" s="48"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="11" t="s">
         <v>50</v>
       </c>
@@ -1794,7 +1850,7 @@
       </c>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C11" s="48"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1803,7 +1859,7 @@
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C12" s="48"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="13" t="s">
         <v>51</v>
       </c>
@@ -1839,7 +1895,7 @@
       <c r="V12" s="5"/>
     </row>
     <row r="13" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C13" s="48"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="13" t="s">
         <v>55</v>
       </c>
@@ -1875,7 +1931,7 @@
       <c r="V13" s="5"/>
     </row>
     <row r="14" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C14" s="48"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="12" t="s">
         <v>56</v>
       </c>
@@ -1911,7 +1967,7 @@
       <c r="V14" s="5"/>
     </row>
     <row r="15" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C15" s="48"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="11" t="s">
         <v>57</v>
       </c>
@@ -1947,7 +2003,7 @@
       <c r="V15" s="5"/>
     </row>
     <row r="16" spans="3:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="C16" s="49"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="11" t="s">
         <v>59</v>
       </c>
@@ -2063,13 +2119,13 @@
       <c r="I19" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="K19" s="44" t="s">
+      <c r="K19" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="L19" s="44" t="s">
+      <c r="L19" s="43" t="s">
         <v>91</v>
       </c>
       <c r="M19" s="5"/>
@@ -2166,7 +2222,7 @@
       <c r="V21" s="5"/>
     </row>
     <row r="22" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="51" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="11" t="s">
@@ -2204,7 +2260,7 @@
       <c r="V22" s="5"/>
     </row>
     <row r="23" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="48"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="16" t="s">
         <v>86</v>
       </c>
@@ -2240,7 +2296,7 @@
       <c r="V23" s="5"/>
     </row>
     <row r="24" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="48"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="16" t="s">
         <v>88</v>
       </c>
@@ -2264,7 +2320,7 @@
       </c>
     </row>
     <row r="25" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="48"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="16" t="s">
         <v>92</v>
       </c>
@@ -2285,7 +2341,7 @@
       </c>
     </row>
     <row r="26" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="49"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="16" t="s">
         <v>96</v>
       </c>
@@ -2360,7 +2416,7 @@
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="51" t="s">
         <v>107</v>
       </c>
       <c r="D31" s="16" t="s">
@@ -2385,7 +2441,7 @@
       </c>
     </row>
     <row r="32" spans="2:31" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="48"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="11" t="s">
         <v>111</v>
       </c>
@@ -2468,7 +2524,7 @@
       </c>
     </row>
     <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="49"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="16" t="s">
         <v>86</v>
       </c>
@@ -2716,7 +2772,7 @@
       <c r="B45" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="51" t="s">
         <v>157</v>
       </c>
       <c r="D45" s="20" t="s">
@@ -2740,7 +2796,7 @@
       </c>
     </row>
     <row r="46" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="48"/>
+      <c r="C46" s="52"/>
       <c r="D46" s="20" t="s">
         <v>163</v>
       </c>
@@ -2762,7 +2818,7 @@
       </c>
     </row>
     <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="49"/>
+      <c r="C47" s="53"/>
       <c r="D47" s="20" t="s">
         <v>166</v>
       </c>

</xml_diff>